<commit_message>
change directory tools into utils, because of the same python build-in package tools
</commit_message>
<xml_diff>
--- a/data/tek_data/GHD_profile.xlsx
+++ b/data/tek_data/GHD_profile.xlsx
@@ -491,9 +491,6 @@
     <t>Kantine</t>
   </si>
   <si>
-    <t>Küche - Vorbereitung, Lager</t>
-  </si>
-  <si>
     <t>Großraumbüro (ab sieben Arbeitsplätze)</t>
   </si>
   <si>
@@ -606,6 +603,9 @@
   </si>
   <si>
     <t>Einzelhandel / Kaufhaus (Lebensmittelabteilung mit Kühlprodukten)</t>
+  </si>
+  <si>
+    <t>Küche – Vorbereitung, Lager</t>
   </si>
 </sst>
 </file>
@@ -3762,7 +3762,7 @@
       <pane xSplit="2" ySplit="1" topLeftCell="H2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B8" sqref="B8"/>
+      <selection pane="bottomRight" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3888,7 +3888,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C3" t="s">
         <v>20</v>
@@ -3938,7 +3938,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>
@@ -4138,7 +4138,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="C8" t="s">
         <v>30</v>
@@ -4188,7 +4188,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C9" t="s">
         <v>24</v>
@@ -4238,7 +4238,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C10" t="s">
         <v>27</v>
@@ -4318,7 +4318,7 @@
         <v>24</v>
       </c>
       <c r="L11" s="6" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M11">
         <v>5</v>
@@ -4488,7 +4488,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C15" s="8" t="s">
         <v>94</v>
@@ -4518,7 +4518,7 @@
         <v>24</v>
       </c>
       <c r="L15" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M15">
         <v>90</v>
@@ -4538,7 +4538,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>129</v>
+        <v>167</v>
       </c>
       <c r="C16" t="s">
         <v>65</v>
@@ -4568,7 +4568,7 @@
         <v>24</v>
       </c>
       <c r="L16" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M16">
         <v>15</v>
@@ -4588,7 +4588,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C17" s="8" t="s">
         <v>75</v>
@@ -4618,19 +4618,19 @@
         <v>24</v>
       </c>
       <c r="L17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M17">
         <v>15</v>
       </c>
       <c r="N17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P17" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
@@ -4638,7 +4638,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C18" s="9" t="s">
         <v>37</v>
@@ -4668,7 +4668,7 @@
         <v>24</v>
       </c>
       <c r="L18" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M18">
         <v>7</v>
@@ -4688,7 +4688,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C19" t="s">
         <v>74</v>
@@ -4718,19 +4718,19 @@
         <v>24</v>
       </c>
       <c r="L19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M19">
         <v>7</v>
       </c>
       <c r="N19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P19" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
@@ -4738,7 +4738,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C20" t="s">
         <v>49</v>
@@ -4768,19 +4768,19 @@
         <v>24</v>
       </c>
       <c r="L20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M20">
         <v>0</v>
       </c>
       <c r="N20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P20" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
@@ -4788,7 +4788,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="C21" t="s">
         <v>45</v>
@@ -4818,19 +4818,19 @@
         <v>24</v>
       </c>
       <c r="L21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M21">
         <v>0.15</v>
       </c>
       <c r="N21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P21" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
@@ -4838,7 +4838,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C22" t="s">
         <v>55</v>
@@ -4885,10 +4885,10 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B23" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C23" t="s">
         <v>43</v>
@@ -4935,10 +4935,10 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
+        <v>140</v>
+      </c>
+      <c r="B24" t="s">
         <v>141</v>
-      </c>
-      <c r="B24" t="s">
-        <v>142</v>
       </c>
       <c r="C24" t="s">
         <v>43</v>
@@ -4985,10 +4985,10 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="6" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B25" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="C25" t="s">
         <v>44</v>
@@ -5038,7 +5038,7 @@
         <v>23</v>
       </c>
       <c r="B26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C26" t="s">
         <v>38</v>
@@ -5080,7 +5080,7 @@
         <v>93</v>
       </c>
       <c r="P26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
@@ -5088,7 +5088,7 @@
         <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C27" t="s">
         <v>39</v>
@@ -5138,7 +5138,7 @@
         <v>25</v>
       </c>
       <c r="B28" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C28" t="s">
         <v>38</v>
@@ -5168,19 +5168,19 @@
         <v>24</v>
       </c>
       <c r="L28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M28">
         <v>0.3</v>
       </c>
       <c r="N28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P28" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
@@ -5188,7 +5188,7 @@
         <v>26</v>
       </c>
       <c r="B29" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C29" t="s">
         <v>38</v>
@@ -5238,7 +5238,7 @@
         <v>27</v>
       </c>
       <c r="B30" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C30" t="s">
         <v>39</v>
@@ -5280,7 +5280,7 @@
         <v>7</v>
       </c>
       <c r="P30" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
@@ -5288,7 +5288,7 @@
         <v>28</v>
       </c>
       <c r="B31" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C31" t="s">
         <v>26</v>
@@ -5330,7 +5330,7 @@
         <v>28</v>
       </c>
       <c r="P31" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
@@ -5338,7 +5338,7 @@
         <v>29</v>
       </c>
       <c r="B32" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C32" t="s">
         <v>26</v>
@@ -5380,7 +5380,7 @@
         <v>7</v>
       </c>
       <c r="P32" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
@@ -5388,7 +5388,7 @@
         <v>30</v>
       </c>
       <c r="B33" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C33" s="8" t="s">
         <v>26</v>
@@ -5418,19 +5418,19 @@
         <v>24</v>
       </c>
       <c r="L33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M33">
         <v>3</v>
       </c>
       <c r="N33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P33" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
@@ -5438,7 +5438,7 @@
         <v>31</v>
       </c>
       <c r="B34" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C34" t="s">
         <v>46</v>
@@ -5480,7 +5480,7 @@
         <v>6.3</v>
       </c>
       <c r="P34" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
@@ -5488,7 +5488,7 @@
         <v>32</v>
       </c>
       <c r="B35" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C35" t="s">
         <v>52</v>
@@ -5518,19 +5518,19 @@
         <v>24</v>
       </c>
       <c r="L35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M35">
         <v>8</v>
       </c>
       <c r="N35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P35" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
@@ -5538,7 +5538,7 @@
         <v>33</v>
       </c>
       <c r="B36" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C36" t="s">
         <v>52</v>
@@ -5568,19 +5568,19 @@
         <v>24</v>
       </c>
       <c r="L36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M36">
         <v>8</v>
       </c>
       <c r="N36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P36" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
@@ -5588,10 +5588,10 @@
         <v>34</v>
       </c>
       <c r="B37" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C37" s="9" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="D37">
         <v>11</v>
@@ -5615,10 +5615,10 @@
         <v>24</v>
       </c>
       <c r="K37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="L37" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M37">
         <v>15</v>
@@ -5688,7 +5688,7 @@
         <v>36</v>
       </c>
       <c r="B39" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C39" s="9" t="s">
         <v>28</v>
@@ -5718,7 +5718,7 @@
         <v>24</v>
       </c>
       <c r="L39" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M39">
         <v>25</v>
@@ -5738,7 +5738,7 @@
         <v>37</v>
       </c>
       <c r="B40" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C40" t="s">
         <v>42</v>
@@ -5768,7 +5768,7 @@
         <v>24</v>
       </c>
       <c r="L40" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M40">
         <v>10</v>
@@ -5788,7 +5788,7 @@
         <v>38</v>
       </c>
       <c r="B41" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C41" t="s">
         <v>41</v>
@@ -5818,7 +5818,7 @@
         <v>24</v>
       </c>
       <c r="L41" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M41">
         <v>30</v>
@@ -5838,7 +5838,7 @@
         <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C42" t="s">
         <v>49</v>
@@ -5868,19 +5868,19 @@
         <v>24</v>
       </c>
       <c r="L42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M42">
         <v>10</v>
       </c>
       <c r="N42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P42" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
@@ -5888,7 +5888,7 @@
         <v>40</v>
       </c>
       <c r="B43" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C43" t="s">
         <v>42</v>
@@ -5918,7 +5918,7 @@
         <v>24</v>
       </c>
       <c r="L43" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="M43">
         <v>10</v>
@@ -5938,7 +5938,7 @@
         <v>41</v>
       </c>
       <c r="B44" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C44" t="s">
         <v>45</v>
@@ -5974,13 +5974,13 @@
         <v>1</v>
       </c>
       <c r="N44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="O44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="P44" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
   </sheetData>

</xml_diff>